<commit_message>
Back UP 14th May
</commit_message>
<xml_diff>
--- a/src/main/java/com/crm/qa/testdata/TestData_Sheet.xlsx
+++ b/src/main/java/com/crm/qa/testdata/TestData_Sheet.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="54">
   <si>
     <t>Title</t>
   </si>
@@ -69,6 +69,120 @@
   </si>
   <si>
     <t>Ebay</t>
+  </si>
+  <si>
+    <t>Pawan1</t>
+  </si>
+  <si>
+    <t>Pawan2</t>
+  </si>
+  <si>
+    <t>Pawan3</t>
+  </si>
+  <si>
+    <t>Pawan4</t>
+  </si>
+  <si>
+    <t>Pawan5</t>
+  </si>
+  <si>
+    <t>Pawan6</t>
+  </si>
+  <si>
+    <t>Pawan7</t>
+  </si>
+  <si>
+    <t>Pawan8</t>
+  </si>
+  <si>
+    <t>Pawan9</t>
+  </si>
+  <si>
+    <t>Pawan10</t>
+  </si>
+  <si>
+    <t>Pawan11</t>
+  </si>
+  <si>
+    <t>Pawan12</t>
+  </si>
+  <si>
+    <t>Pawan13</t>
+  </si>
+  <si>
+    <t>Pawan14</t>
+  </si>
+  <si>
+    <t>Pawan15</t>
+  </si>
+  <si>
+    <t>Pawan16</t>
+  </si>
+  <si>
+    <t>Pawan17</t>
+  </si>
+  <si>
+    <t>Pawan18</t>
+  </si>
+  <si>
+    <t>Pawan19</t>
+  </si>
+  <si>
+    <t>Awasthi1</t>
+  </si>
+  <si>
+    <t>Awasthi2</t>
+  </si>
+  <si>
+    <t>Awasthi3</t>
+  </si>
+  <si>
+    <t>Awasthi4</t>
+  </si>
+  <si>
+    <t>Awasthi5</t>
+  </si>
+  <si>
+    <t>Awasthi6</t>
+  </si>
+  <si>
+    <t>Awasthi7</t>
+  </si>
+  <si>
+    <t>Awasthi8</t>
+  </si>
+  <si>
+    <t>Awasthi9</t>
+  </si>
+  <si>
+    <t>Awasthi10</t>
+  </si>
+  <si>
+    <t>Awasthi11</t>
+  </si>
+  <si>
+    <t>Awasthi12</t>
+  </si>
+  <si>
+    <t>Awasthi13</t>
+  </si>
+  <si>
+    <t>Awasthi14</t>
+  </si>
+  <si>
+    <t>Awasthi15</t>
+  </si>
+  <si>
+    <t>Awasthi16</t>
+  </si>
+  <si>
+    <t>Awasthi17</t>
+  </si>
+  <si>
+    <t>Awasthi18</t>
+  </si>
+  <si>
+    <t>Awasthi19</t>
   </si>
 </sst>
 </file>
@@ -386,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -413,10 +527,10 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
@@ -427,10 +541,10 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="D3" t="s">
         <v>12</v>
@@ -441,12 +555,236 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="D4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>